<commit_message>
CI list - adding links
</commit_message>
<xml_diff>
--- a/Documents/Configuration Items List v4.1.xlsx
+++ b/Documents/Configuration Items List v4.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>Configuration Item Name</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Bugs</t>
   </si>
   <si>
-    <t>PivotalTracker</t>
-  </si>
-  <si>
     <t>Issues from Peer Reviews retained</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>UML - Use Cases</t>
-  </si>
-  <si>
     <t>UML - Components Diagram</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>Mocks ups/Wireframes</t>
   </si>
   <si>
-    <t>Balsamiq/GitHub</t>
-  </si>
-  <si>
     <t>Estimation Record</t>
   </si>
   <si>
@@ -125,6 +116,12 @@
   </si>
   <si>
     <t>Definition of Scope and Team Compositions</t>
+  </si>
+  <si>
+    <t>Use Case UML</t>
+  </si>
+  <si>
+    <t>Loans and Grants Website</t>
   </si>
 </sst>
 </file>
@@ -134,7 +131,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,15 +175,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -352,6 +340,15 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -361,17 +358,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -678,7 +666,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,13 +681,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -715,7 +703,7 @@
       <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -724,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -732,10 +720,10 @@
       <c r="D3" s="5">
         <v>42141</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="E3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -755,7 +743,7 @@
       <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -775,7 +763,7 @@
       <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -784,10 +772,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D6" s="5">
         <v>42162</v>
@@ -795,7 +783,7 @@
       <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -804,7 +792,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4">
         <v>2</v>
@@ -815,7 +803,7 @@
       <c r="E7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -824,7 +812,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4">
         <v>2</v>
@@ -835,7 +823,7 @@
       <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -844,7 +832,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -855,7 +843,7 @@
       <c r="E9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -864,7 +852,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4">
         <v>2.2999999999999998</v>
@@ -875,7 +863,7 @@
       <c r="E10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -895,16 +883,14 @@
       <c r="E11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="4">
         <v>2</v>
@@ -915,8 +901,8 @@
       <c r="E12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>31</v>
+      <c r="F12" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -924,7 +910,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4">
         <v>1.2</v>
@@ -935,7 +921,7 @@
       <c r="E13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1035,7 +1021,7 @@
       <c r="E18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1055,8 +1041,8 @@
       <c r="E19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>6</v>
+      <c r="F19" s="12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1067,7 +1053,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="5">
         <v>42157</v>
@@ -1087,7 +1073,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="5">
         <v>42174</v>
@@ -1095,8 +1081,8 @@
       <c r="E21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>23</v>
+      <c r="F21" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1104,10 +1090,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="5">
         <v>42174</v>
@@ -1115,7 +1101,7 @@
       <c r="E22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1127,8 +1113,19 @@
     <hyperlink ref="F3" r:id="rId1" display="https://github.com/wshahzad/Team-Four/blob/master/Documents/Project Proposal and Team Composition.docx"/>
     <hyperlink ref="F4" r:id="rId2"/>
     <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6"/>
+    <hyperlink ref="F9" r:id="rId7"/>
+    <hyperlink ref="F10" r:id="rId8"/>
+    <hyperlink ref="F12" r:id="rId9"/>
+    <hyperlink ref="F13" r:id="rId10"/>
+    <hyperlink ref="F18" r:id="rId11"/>
+    <hyperlink ref="F19" r:id="rId12"/>
+    <hyperlink ref="F21" r:id="rId13"/>
+    <hyperlink ref="F22" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>